<commit_message>
ERC, Div, Log, much harder target function, code cleanup
</commit_message>
<xml_diff>
--- a/GeneticProgrammingPortfolio/testinput.xlsx
+++ b/GeneticProgrammingPortfolio/testinput.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\GitHub\GPP\GeneticProgrammingPortfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesEarle\Documents\Development\GitHub\GPP\GeneticProgrammingPortfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -336,21 +336,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
-        <f>A1 * A1 + 3 * A1 + 10</f>
-        <v>14</v>
+        <f xml:space="preserve"> 3.14 * A1 * A1 * A1 + 7.6 + A1 - 2 * A1 / 13 + 12 - A1 * A1</f>
+        <v>22.586153846153849</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -358,8 +361,8 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B10" si="0">A2 * A2 + 3 * A2 + 10</f>
-        <v>20</v>
+        <f t="shared" ref="B2:B65" si="0" xml:space="preserve"> 3.14 * A2 * A2 * A2 + 7.6 + A2 - 2 * A2 / 13 + 12 - A2 * A2</f>
+        <v>42.412307692307692</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -368,7 +371,7 @@
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>97.918461538461528</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -377,7 +380,7 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>207.94461538461539</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -386,7 +389,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>391.33076923076925</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -395,7 +398,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>666.91692307692313</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -404,7 +407,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>1053.5430769230768</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -413,7 +416,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>98</v>
+        <v>1570.0492307692307</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -422,7 +425,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>118</v>
+        <v>2235.2753846153846</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -431,7 +434,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>3068.0615384615385</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -439,8 +442,8 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <f t="shared" ref="B11:B25" si="1">A11 * A11 + 3 * A11 + 10</f>
-        <v>164</v>
+        <f t="shared" si="0"/>
+        <v>4087.2476923076929</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -448,8 +451,8 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
-        <v>190</v>
+        <f t="shared" si="0"/>
+        <v>5311.6738461538462</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -457,8 +460,8 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
-        <v>218</v>
+        <f t="shared" si="0"/>
+        <v>6760.18</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -466,8 +469,8 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
-        <v>248</v>
+        <f t="shared" si="0"/>
+        <v>8451.6061538461545</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -475,8 +478,8 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
-        <v>280</v>
+        <f t="shared" si="0"/>
+        <v>10404.792307692309</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,8 +487,8 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
-        <v>314</v>
+        <f t="shared" si="0"/>
+        <v>12638.578461538462</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -493,8 +496,8 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
-        <v>350</v>
+        <f t="shared" si="0"/>
+        <v>15171.804615384615</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -502,8 +505,8 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
-        <v>388</v>
+        <f t="shared" si="0"/>
+        <v>18023.310769230768</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -511,8 +514,8 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
-        <v>428</v>
+        <f t="shared" si="0"/>
+        <v>21211.936923076919</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -520,8 +523,8 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
-        <v>470</v>
+        <f t="shared" si="0"/>
+        <v>24756.523076923077</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -529,8 +532,8 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
-        <v>514</v>
+        <f t="shared" si="0"/>
+        <v>28675.90923076923</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -538,8 +541,8 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
-        <v>560</v>
+        <f t="shared" si="0"/>
+        <v>32988.935384615383</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -547,8 +550,8 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
-        <v>608</v>
+        <f t="shared" si="0"/>
+        <v>37714.441538461535</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -556,8 +559,8 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
-        <v>658</v>
+        <f t="shared" si="0"/>
+        <v>42871.267692307694</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -565,8 +568,683 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <f>A25 * A25 + 3 * A25 + 10</f>
-        <v>710</v>
+        <f t="shared" si="0"/>
+        <v>48478.253846153842</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>54554.239999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>61118.06615384615</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>68188.572307692317</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>75784.59846153848</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>83924.984615384616</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>92628.570769230777</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>101914.19692307693</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>111800.70307692309</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>122306.92923076924</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>133451.71538461538</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>145253.90153846153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>157732.32769230768</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>170905.83384615384</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>184793.26000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>199413.44615384616</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>214785.23230769232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>230927.45846153848</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>247858.96461538467</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>265598.59076923074</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>284165.17692307697</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>303577.56307692302</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>323854.58923076926</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>345015.09538461536</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>367077.92153846158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>390061.90769230766</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>413985.89384615386</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>438868.72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>464729.22615384613</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>491586.25230769225</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>519458.63846153853</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>548365.22461538459</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>578324.85076923075</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>609356.35692307691</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>641478.58307692327</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>674710.36923076923</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>709070.55538461544</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>744577.98153846152</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>781251.4876923078</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>64</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>819109.91384615388</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>65</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>858172.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>66</v>
+      </c>
+      <c r="B66">
+        <f t="shared" ref="B66:B100" si="1" xml:space="preserve"> 3.14 * A66 * A66 * A66 + 7.6 + A66 - 2 * A66 / 13 + 12 - A66 * A66</f>
+        <v>898456.88615384616</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="1"/>
+        <v>939983.11230769218</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>68</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="1"/>
+        <v>982769.61846153846</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>69</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="1"/>
+        <v>1026835.2446153845</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>70</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="1"/>
+        <v>1072198.8307692308</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>71</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="1"/>
+        <v>1118879.2169230771</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>1166895.2430769231</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>73</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>1216265.7492307695</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>74</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="1"/>
+        <v>1267009.5753846155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>75</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="1"/>
+        <v>1319145.5615384616</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>76</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="1"/>
+        <v>1372692.5476923077</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>77</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="1"/>
+        <v>1427669.373846154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>78</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="1"/>
+        <v>1484094.8800000004</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="1"/>
+        <v>1541987.9061538465</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>80</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="1"/>
+        <v>1601367.2923076923</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>81</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="1"/>
+        <v>1662251.8784615386</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>82</v>
+      </c>
+      <c r="B82">
+        <f t="shared" si="1"/>
+        <v>1724660.5046153846</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>83</v>
+      </c>
+      <c r="B83">
+        <f t="shared" si="1"/>
+        <v>1788612.0107692308</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>84</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="1"/>
+        <v>1854125.2369230771</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>85</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="1"/>
+        <v>1921219.0230769233</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>86</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="1"/>
+        <v>1989912.2092307697</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>87</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="1"/>
+        <v>2060223.6353846155</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="1"/>
+        <v>2132172.1415384617</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89">
+        <f t="shared" si="1"/>
+        <v>2205776.5676923078</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90">
+        <f t="shared" si="1"/>
+        <v>2281055.7538461545</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91">
+        <f t="shared" si="1"/>
+        <v>2358028.54</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>92</v>
+      </c>
+      <c r="B92">
+        <f t="shared" si="1"/>
+        <v>2436713.7661538459</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>93</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="1"/>
+        <v>2517130.272307693</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>94</v>
+      </c>
+      <c r="B94">
+        <f t="shared" si="1"/>
+        <v>2599296.8984615388</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>95</v>
+      </c>
+      <c r="B95">
+        <f t="shared" si="1"/>
+        <v>2683232.4846153846</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>96</v>
+      </c>
+      <c r="B96">
+        <f t="shared" si="1"/>
+        <v>2768955.8707692311</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>97</v>
+      </c>
+      <c r="B97">
+        <f t="shared" si="1"/>
+        <v>2856485.8969230768</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>98</v>
+      </c>
+      <c r="B98">
+        <f t="shared" si="1"/>
+        <v>2945841.4030769235</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>99</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="1"/>
+        <v>3037041.2292307694</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>100</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="1"/>
+        <v>3130104.2153846156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>